<commit_message>
modded package.json to run nodemon instead on npm start, map.js can now switch between data of different timestamps, added date select to index.html
</commit_message>
<xml_diff>
--- a/Data/Working with Worldview Data/firedata_Indon_2Sept2019.xlsx
+++ b/Data/Working with Worldview Data/firedata_Indon_2Sept2019.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deSni\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deSni\OneDrive\Code practice\NASAHackathon\GoogleMapsNChartTestbed\Data\Working with Worldview Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>lat</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>Time scale: September 2, 1 day average</t>
+  </si>
+  <si>
+    <t>Random generator:</t>
   </si>
 </sst>
 </file>
@@ -92,8 +95,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -374,18 +378,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="6" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -398,8 +403,11 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>-7.1135077000000004</v>
       </c>
@@ -412,11 +420,19 @@
       <c r="D2">
         <v>51</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1">
+        <f ca="1">C2*RAND()*(1-0.01)</f>
+        <v>7.0063730849570609</v>
+      </c>
+      <c r="G2" s="1">
+        <f t="shared" ref="G2:G28" ca="1" si="0">D2*RAND()*(1-0.01)</f>
+        <v>29.860533954887131</v>
+      </c>
+      <c r="M2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>-6.6392699999999998</v>
       </c>
@@ -429,11 +445,19 @@
       <c r="D3">
         <v>72</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1">
+        <f t="shared" ref="F3:F28" ca="1" si="1">C3*RAND()*(1-0.01)</f>
+        <v>7.9644601294194191</v>
+      </c>
+      <c r="G3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>8.9082479546195366</v>
+      </c>
+      <c r="M3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>-6.6356726000000004</v>
       </c>
@@ -446,8 +470,16 @@
       <c r="D4">
         <v>74</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F4" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>11.730801340426973</v>
+      </c>
+      <c r="G4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>71.234579101929299</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>-5.4917009999999999</v>
       </c>
@@ -460,11 +492,19 @@
       <c r="D5">
         <v>61</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>12.478437993804608</v>
+      </c>
+      <c r="G5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>27.348157328957473</v>
+      </c>
+      <c r="M5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>-5.4914864999999997</v>
       </c>
@@ -477,11 +517,19 @@
       <c r="D6">
         <v>65</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>26.179424387752636</v>
+      </c>
+      <c r="G6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.343818580974494</v>
+      </c>
+      <c r="M6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>-5.4366950000000003</v>
       </c>
@@ -494,8 +542,16 @@
       <c r="D7">
         <v>57</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>2.7516045496495636E-2</v>
+      </c>
+      <c r="G7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>34.505704992384594</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>-3.1169574</v>
       </c>
@@ -508,11 +564,19 @@
       <c r="D8">
         <v>64</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>18.835093024907835</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>38.925312099368384</v>
+      </c>
+      <c r="M8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>-2.0214070999999998</v>
       </c>
@@ -525,11 +589,19 @@
       <c r="D9">
         <v>54</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>3.8924507970404507</v>
+      </c>
+      <c r="G9" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>14.42387610969412</v>
+      </c>
+      <c r="M9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>-1.2726766</v>
       </c>
@@ -542,11 +614,19 @@
       <c r="D10">
         <v>21</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>32.120101170951216</v>
+      </c>
+      <c r="G10" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.7749435121600792</v>
+      </c>
+      <c r="M10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>-1.2877399</v>
       </c>
@@ -559,8 +639,16 @@
       <c r="D11">
         <v>63</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F11" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>42.219385935237057</v>
+      </c>
+      <c r="G11" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>44.02252810696104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>-1.0831339</v>
       </c>
@@ -573,8 +661,16 @@
       <c r="D12">
         <v>61</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F12" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>2.493897627248348</v>
+      </c>
+      <c r="G12" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>33.996835564075411</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>-0.86079276000000005</v>
       </c>
@@ -587,8 +683,16 @@
       <c r="D13">
         <v>63</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F13" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>11.942114838700491</v>
+      </c>
+      <c r="G13" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>53.342763596772585</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>-0.14272620999999999</v>
       </c>
@@ -601,8 +705,16 @@
       <c r="D14">
         <v>60</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F14" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>2.0230181007565298</v>
+      </c>
+      <c r="G14" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>9.5886454959145926</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1.9170731000000001</v>
       </c>
@@ -615,8 +727,16 @@
       <c r="D15">
         <v>61</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F15" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>10.667729458201858</v>
+      </c>
+      <c r="G15" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>46.340926033995629</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1.9297986</v>
       </c>
@@ -629,8 +749,16 @@
       <c r="D16">
         <v>74</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F16" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>4.1375709240359928</v>
+      </c>
+      <c r="G16" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>72.181374134972131</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1.9049971000000001</v>
       </c>
@@ -643,8 +771,16 @@
       <c r="D17">
         <v>53</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F17" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>3.9784442675984817</v>
+      </c>
+      <c r="G17" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>44.442506357834993</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1.9031591000000001</v>
       </c>
@@ -657,8 +793,16 @@
       <c r="D18">
         <v>85</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F18" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>22.906433573084076</v>
+      </c>
+      <c r="G18" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>60.921826772481232</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1.9137803</v>
       </c>
@@ -671,8 +815,16 @@
       <c r="D19">
         <v>59</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F19" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>13.688778334793504</v>
+      </c>
+      <c r="G19" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>28.181058099533956</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2.0588622000000001</v>
       </c>
@@ -685,8 +837,16 @@
       <c r="D20">
         <v>91</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F20" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>54.271352528722716</v>
+      </c>
+      <c r="G20" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>38.260522042736561</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2.0570376000000001</v>
       </c>
@@ -699,8 +859,16 @@
       <c r="D21">
         <v>100</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F21" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>56.731937443049759</v>
+      </c>
+      <c r="G21" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>90.662019136168865</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2.7017934000000001</v>
       </c>
@@ -713,8 +881,16 @@
       <c r="D22">
         <v>80</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F22" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>42.065026538770994</v>
+      </c>
+      <c r="G22" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>30.768318191552446</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2.6995309999999999</v>
       </c>
@@ -727,8 +903,16 @@
       <c r="D23">
         <v>78</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F23" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>15.286404368466558</v>
+      </c>
+      <c r="G23" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>47.047974789977395</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2.8778508</v>
       </c>
@@ -741,8 +925,16 @@
       <c r="D24">
         <v>70</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F24" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>1.2789994368127038</v>
+      </c>
+      <c r="G24" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>26.372763021009277</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>3.4250286000000001</v>
       </c>
@@ -755,8 +947,16 @@
       <c r="D25">
         <v>48</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F25" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>16.593501334638432</v>
+      </c>
+      <c r="G25" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>31.942581716186858</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>3.5281413000000001</v>
       </c>
@@ -769,8 +969,16 @@
       <c r="D26">
         <v>66</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F26" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>2.6794877613153392</v>
+      </c>
+      <c r="G26" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45.204117803709146</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>4.019469</v>
       </c>
@@ -783,8 +991,16 @@
       <c r="D27">
         <v>43</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F27" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.96012172617188452</v>
+      </c>
+      <c r="G27" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>8.562136903631437</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>4.4212436999999998</v>
       </c>
@@ -796,6 +1012,14 @@
       </c>
       <c r="D28">
         <v>77</v>
+      </c>
+      <c r="F28" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>4.4186020221500257</v>
+      </c>
+      <c r="G28" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>16.734232516263926</v>
       </c>
     </row>
   </sheetData>

</xml_diff>